<commit_message>
refactored way data is read, added bayes filtercore steps
</commit_message>
<xml_diff>
--- a/Lab2/E205_Lab2_NuScenesData.xlsx
+++ b/Lab2/E205_Lab2_NuScenesData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter Johnson\Desktop\E205\Lab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163D3ACB-8754-DA48-A07E-4AAB7323C184}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D7A2E5-C2C4-4345-84F0-D3C0C2BF7D36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="1840" windowWidth="14400" windowHeight="17540" xr2:uid="{DA864444-5E00-5448-9391-4E45375BE65B}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{DA864444-5E00-5448-9391-4E45375BE65B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -586,10 +586,10 @@
   <dimension ref="A1:V41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" t="s">

</xml_diff>